<commit_message>
Primeira automação na versão um, onde ocorre um teste no login e na pesquisa de um filme
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felipe.almeida\Documents\java-workspace\Netflix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EE53B9-77E5-4839-A370-351F58B8DF0C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A523946-D3B1-4715-96AF-AC11A6106139}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14490" yWindow="1200" windowWidth="11520" windowHeight="7875" xr2:uid="{17B324B1-8A02-4A8A-BDC9-F5E2761017EE}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{17B324B1-8A02-4A8A-BDC9-F5E2761017EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>CasoDeTeste nº</t>
   </si>
@@ -39,50 +39,37 @@
     <t>e-mail</t>
   </si>
   <si>
-    <t>gabriella.cristinec@gmail.com</t>
-  </si>
-  <si>
-    <t>jose.roberto@live.com</t>
-  </si>
-  <si>
     <t>senha</t>
   </si>
   <si>
-    <t>gabi2209</t>
-  </si>
-  <si>
-    <t>gustavooooo@</t>
-  </si>
-  <si>
-    <t>gerome</t>
-  </si>
-  <si>
     <t>filmePesquisa</t>
   </si>
   <si>
-    <t>papai noel</t>
-  </si>
-  <si>
-    <t>the witcher</t>
-  </si>
-  <si>
     <t>Resultado</t>
   </si>
   <si>
-    <t>felipe.cortez@ggg.com</t>
-  </si>
-  <si>
-    <t>Passou</t>
-  </si>
-  <si>
-    <t>esquadrao 6</t>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>user3</t>
+  </si>
+  <si>
+    <t>filme 1</t>
+  </si>
+  <si>
+    <t>filme 2</t>
+  </si>
+  <si>
+    <t>filme 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -452,11 +439,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="28.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="29.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -467,13 +454,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -481,13 +468,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="C2" s="1">
+        <v>123</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -495,10 +482,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="C3" s="3">
+        <v>123</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
@@ -509,16 +496,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="3">
+        <v>123</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>